<commit_message>
Updated version of pi code
</commit_message>
<xml_diff>
--- a/Packet_Layout_SQLite_Sensor_Pinout V.1.xlsx
+++ b/Packet_Layout_SQLite_Sensor_Pinout V.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimke\OneDrive\Documents\GitHub\FSAE2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120B6931-8B19-40BF-8A93-7D3DF0A272E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D33D23-7E85-4C7A-8A51-94471C1881C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{B0CF7E5F-438D-42C7-92ED-3F2500AC4C9B}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{B0CF7E5F-438D-42C7-92ED-3F2500AC4C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="LoRa Packet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="197">
   <si>
     <t>Name</t>
   </si>
@@ -626,6 +626,9 @@
   </si>
   <si>
     <t>Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0000000000</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1045,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1131,6 +1134,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1140,66 +1181,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1585,7 +1570,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection sqref="A1:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,7 +1608,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="48" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1646,7 +1631,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1667,7 +1652,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1688,7 +1673,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1709,7 +1694,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="48" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1732,7 +1717,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1753,7 +1738,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1774,7 +1759,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1795,7 +1780,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="48" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1818,7 +1803,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1839,7 +1824,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1860,7 +1845,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1881,7 +1866,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="48" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1904,7 +1889,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1925,7 +1910,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1946,7 +1931,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1967,7 +1952,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="48" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1990,7 +1975,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
@@ -2011,7 +1996,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
@@ -2032,7 +2017,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
@@ -2053,7 +2038,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="48" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -2076,7 +2061,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="2" t="s">
         <v>26</v>
       </c>
@@ -2097,7 +2082,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
@@ -2118,28 +2103,28 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44"/>
-      <c r="B25" s="53" t="s">
+      <c r="A25" s="51"/>
+      <c r="B25" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="F25" s="45" t="s">
+      <c r="F25" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="46" t="s">
+      <c r="G25" s="38" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="48" t="s">
         <v>80</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -2162,7 +2147,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="8" t="s">
         <v>78</v>
       </c>
@@ -2183,7 +2168,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="9" t="s">
         <v>79</v>
       </c>
@@ -2204,10 +2189,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="7" t="s">
         <v>183</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -2227,8 +2212,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="39" t="s">
+      <c r="A30" s="46"/>
+      <c r="B30" s="8" t="s">
         <v>185</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -2237,7 +2222,7 @@
       <c r="D30" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E30" s="52" t="s">
+      <c r="E30" s="39" t="s">
         <v>189</v>
       </c>
       <c r="F30" s="12">
@@ -2248,8 +2233,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="50"/>
-      <c r="B31" s="51" t="s">
+      <c r="A31" s="47"/>
+      <c r="B31" s="9" t="s">
         <v>184</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -2258,7 +2243,7 @@
       <c r="D31" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="42" t="s">
         <v>189</v>
       </c>
       <c r="F31" s="13">
@@ -2271,52 +2256,55 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32" s="18"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="18"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="18"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="18"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="18"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D38" s="18"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D39" s="18"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D41" s="18"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D42" s="18"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D43" s="18"/>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="G43" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D44" s="18"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D45" s="18"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D46" s="18"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D47" s="18"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D48" s="18"/>
     </row>
   </sheetData>
@@ -2340,7 +2328,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="C30" sqref="A1:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,13 +2339,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="43" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2368,7 +2356,7 @@
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="44" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2379,7 +2367,7 @@
       <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2390,7 +2378,7 @@
       <c r="B4" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2401,7 +2389,7 @@
       <c r="B5" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2412,7 +2400,7 @@
       <c r="B6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2423,7 +2411,7 @@
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2434,7 +2422,7 @@
       <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2445,7 +2433,7 @@
       <c r="B9" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2456,7 +2444,7 @@
       <c r="B10" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2467,7 +2455,7 @@
       <c r="B11" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2478,7 +2466,7 @@
       <c r="B12" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2489,7 +2477,7 @@
       <c r="B13" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2500,7 +2488,7 @@
       <c r="B14" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="57" t="s">
+      <c r="C14" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2511,7 +2499,7 @@
       <c r="B15" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2522,7 +2510,7 @@
       <c r="B16" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2533,7 +2521,7 @@
       <c r="B17" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2544,7 +2532,7 @@
       <c r="B18" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2555,7 +2543,7 @@
       <c r="B19" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2566,7 +2554,7 @@
       <c r="B20" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2577,7 +2565,7 @@
       <c r="B21" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2588,7 +2576,7 @@
       <c r="B22" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2599,7 +2587,7 @@
       <c r="B23" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2610,7 +2598,7 @@
       <c r="B24" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C24" s="57" t="s">
+      <c r="C24" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2621,7 +2609,7 @@
       <c r="B25" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2632,52 +2620,52 @@
       <c r="B26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="44" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C30" s="17" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C28" s="57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C29" s="57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="43" t="s">
-        <v>184</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="C30" s="58" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2692,7 +2680,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2703,11 +2691,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -2851,11 +2839,11 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2990,10 +2978,10 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="B31" s="38"/>
+      <c r="B31" s="52"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">

</xml_diff>

<commit_message>
Edits for bringing car online
</commit_message>
<xml_diff>
--- a/Packet_Layout_SQLite_Sensor_Pinout V.1.xlsx
+++ b/Packet_Layout_SQLite_Sensor_Pinout V.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimke\OneDrive\Documents\GitHub\FSAE2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cs320-spring2022\CS320_Lab02a_jkeller11\FSAE2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687896C4-0CD1-4FF5-8AD2-3A94058284DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA8A84-3C9E-4284-98B0-82B326381EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{B0CF7E5F-438D-42C7-92ED-3F2500AC4C9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B0CF7E5F-438D-42C7-92ED-3F2500AC4C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="LoRa Packet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="186">
   <si>
     <t>Name</t>
   </si>
@@ -589,40 +589,7 @@
     <t>Chained Neopixels  GPIO 24</t>
   </si>
   <si>
-    <t>Lambda #1 Measured</t>
-  </si>
-  <si>
-    <t>Target Lambda</t>
-  </si>
-  <si>
-    <t>Lambda #2 Measured</t>
-  </si>
-  <si>
-    <t>Lambda_1</t>
-  </si>
-  <si>
-    <t>Lambda_2</t>
-  </si>
-  <si>
-    <t>Target_Lambda</t>
-  </si>
-  <si>
     <t>Int</t>
-  </si>
-  <si>
-    <t>0 - 10</t>
-  </si>
-  <si>
-    <t>0 - 2.5</t>
-  </si>
-  <si>
-    <t>50 - 51</t>
-  </si>
-  <si>
-    <t>52 - 53</t>
-  </si>
-  <si>
-    <t>54 - 55</t>
   </si>
   <si>
     <t>Timestamp</t>
@@ -635,7 +602,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -688,14 +655,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -717,7 +676,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1015,37 +974,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1147,30 +1080,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1567,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DAB823-AFF8-4800-B8FA-5A3E7835B793}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G31"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1526,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="43" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1631,7 +1549,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1652,7 +1570,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1673,7 +1591,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1694,7 +1612,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="43" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1717,7 +1635,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1738,7 +1656,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1759,7 +1677,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1770,7 +1688,7 @@
         <v>126</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>39</v>
@@ -1780,7 +1698,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="43" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1803,7 +1721,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1824,7 +1742,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1845,7 +1763,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1866,7 +1784,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1889,7 +1807,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1910,7 +1828,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1931,7 +1849,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1952,7 +1870,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="43" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1975,7 +1893,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1996,7 +1914,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
@@ -2017,7 +1935,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
+      <c r="A21" s="45"/>
       <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
@@ -2038,7 +1956,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="43" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -2061,7 +1979,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="2" t="s">
         <v>26</v>
       </c>
@@ -2082,7 +2000,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
@@ -2103,18 +2021,18 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
-      <c r="B25" s="40" t="s">
+      <c r="A25" s="46"/>
+      <c r="B25" s="39" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D25" s="40" t="s">
         <v>126</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F25" s="37" t="s">
         <v>39</v>
@@ -2124,7 +2042,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="43" t="s">
         <v>80</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -2147,7 +2065,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="8" t="s">
         <v>78</v>
       </c>
@@ -2168,7 +2086,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="50"/>
+      <c r="A28" s="45"/>
       <c r="B28" s="9" t="s">
         <v>79</v>
       </c>
@@ -2188,70 +2106,14 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="F29" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>190</v>
-      </c>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="F30" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="47"/>
-      <c r="B31" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E31" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="F31" s="13">
-        <v>0.01</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>191</v>
-      </c>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="18"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32" s="18"/>
@@ -2279,6 +2141,9 @@
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D40" s="18"/>
+      <c r="G40" s="18" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D41" s="18"/>
@@ -2288,9 +2153,6 @@
     </row>
     <row r="43" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D43" s="18"/>
-      <c r="G43" s="18" t="s">
-        <v>196</v>
-      </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D44" s="18"/>
@@ -2298,18 +2160,8 @@
     <row r="45" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D45" s="18"/>
     </row>
-    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D46" s="18"/>
-    </row>
-    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="18"/>
-    </row>
-    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D48" s="18"/>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A29:A31"/>
+  <mergeCells count="7">
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
@@ -2325,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18402DEB-E4E0-4F86-9553-AF55B8C5ECBF}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,7 +2197,7 @@
       <c r="B1" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="41" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2356,7 +2208,7 @@
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="42" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2367,7 +2219,7 @@
       <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2378,7 +2230,7 @@
       <c r="B4" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2389,7 +2241,7 @@
       <c r="B5" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2400,7 +2252,7 @@
       <c r="B6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2411,7 +2263,7 @@
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2422,7 +2274,7 @@
       <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2433,7 +2285,7 @@
       <c r="B9" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2444,7 +2296,7 @@
       <c r="B10" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2455,7 +2307,7 @@
       <c r="B11" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2466,7 +2318,7 @@
       <c r="B12" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2477,7 +2329,7 @@
       <c r="B13" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2488,7 +2340,7 @@
       <c r="B14" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2499,7 +2351,7 @@
       <c r="B15" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2510,7 +2362,7 @@
       <c r="B16" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2521,7 +2373,7 @@
       <c r="B17" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2532,7 +2384,7 @@
       <c r="B18" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2543,7 +2395,7 @@
       <c r="B19" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2554,7 +2406,7 @@
       <c r="B20" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2565,7 +2417,7 @@
       <c r="B21" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2576,7 +2428,7 @@
       <c r="B22" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2587,7 +2439,7 @@
       <c r="B23" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2598,7 +2450,7 @@
       <c r="B24" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2609,7 +2461,7 @@
       <c r="B25" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2620,52 +2472,19 @@
       <c r="B26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="42" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C28" s="44" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>195</v>
+      <c r="B27" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2691,11 +2510,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -2839,11 +2658,11 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2978,10 +2797,10 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="B31" s="52"/>
+      <c r="B31" s="47"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">

</xml_diff>

<commit_message>
Removed Data from LoRa Packet
</commit_message>
<xml_diff>
--- a/Packet_Layout_SQLite_Sensor_Pinout V.1.xlsx
+++ b/Packet_Layout_SQLite_Sensor_Pinout V.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cs320-spring2022\CS320_Lab02a_jkeller11\FSAE2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D5BFA5-9626-48D8-85D0-3B78287CA735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED0BB1D-C128-46E7-B41E-21E2EB69879E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="16020" windowHeight="15585" activeTab="1" xr2:uid="{B0CF7E5F-438D-42C7-92ED-3F2500AC4C9B}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{B0CF7E5F-438D-42C7-92ED-3F2500AC4C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="LoRa Packet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="189">
   <si>
     <t>Name</t>
   </si>
@@ -596,6 +596,15 @@
   </si>
   <si>
     <t>Steering angle / Analog 7</t>
+  </si>
+  <si>
+    <t>50-51</t>
+  </si>
+  <si>
+    <t>52-53</t>
+  </si>
+  <si>
+    <t>Position in Raspi code</t>
   </si>
 </sst>
 </file>
@@ -682,7 +691,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -991,11 +1000,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1045,9 +1063,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1098,13 +1113,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1122,9 +1144,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1505,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DAB823-AFF8-4800-B8FA-5A3E7835B793}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,13 +1550,14 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -1532,7 +1567,7 @@
       <c r="C1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="51" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
@@ -1544,9 +1579,12 @@
       <c r="G1" s="14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="H1" s="42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1555,7 +1593,7 @@
       <c r="C2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -1567,16 +1605,19 @@
       <c r="G2" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
+      <c r="H2" s="43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="46"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="8" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="12" t="s">
@@ -1588,16 +1629,19 @@
       <c r="G3" s="16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+      <c r="H3" s="43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="46"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="8" t="s">
         <v>54</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -1609,17 +1653,20 @@
       <c r="G4" s="16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="49" t="s">
+      <c r="H4" s="43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="47"/>
+      <c r="B5" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>55</v>
+      <c r="D5" s="52" t="s">
+        <v>119</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>37</v>
@@ -1630,19 +1677,22 @@
       <c r="G5" s="17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="H5" s="44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="50" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>56</v>
+      <c r="D6" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>37</v>
@@ -1653,17 +1703,20 @@
       <c r="G6" s="15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="H6" s="43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>57</v>
+      <c r="D7" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>37</v>
@@ -1674,17 +1727,20 @@
       <c r="G7" s="16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="2" t="s">
+      <c r="H7" s="43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="46"/>
+      <c r="B8" s="56" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>58</v>
+      <c r="D8" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>37</v>
@@ -1695,16 +1751,19 @@
       <c r="G8" s="16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
+      <c r="H8" s="43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="47"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="52" t="s">
         <v>119</v>
       </c>
       <c r="E9" s="13" t="s">
@@ -1716,19 +1775,22 @@
       <c r="G9" s="17" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="H9" s="44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="50" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>59</v>
+      <c r="D10" s="54" t="s">
+        <v>119</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>37</v>
@@ -1739,17 +1801,20 @@
       <c r="G10" s="15" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="H10" s="43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="46"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>60</v>
+      <c r="D11" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>37</v>
@@ -1760,17 +1825,20 @@
       <c r="G11" s="16" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="H11" s="43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="46"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>61</v>
+      <c r="D12" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>37</v>
@@ -1781,17 +1849,20 @@
       <c r="G12" s="16" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+      <c r="H12" s="43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="47"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>62</v>
+      <c r="D13" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>37</v>
@@ -1802,9 +1873,12 @@
       <c r="G13" s="17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="H13" s="43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="45" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1813,8 +1887,8 @@
       <c r="C14" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>63</v>
+      <c r="D14" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>37</v>
@@ -1825,17 +1899,20 @@
       <c r="G14" s="15" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="H14" s="43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="46"/>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>64</v>
+      <c r="D15" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>37</v>
@@ -1846,17 +1923,20 @@
       <c r="G15" s="16" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
+      <c r="H15" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="46"/>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>65</v>
+      <c r="D16" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>37</v>
@@ -1867,17 +1947,20 @@
       <c r="G16" s="16" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45"/>
-      <c r="B17" s="49" t="s">
+      <c r="H16" s="43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47"/>
+      <c r="B17" s="55" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>66</v>
+      <c r="D17" s="52" t="s">
+        <v>119</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>37</v>
@@ -1888,9 +1971,12 @@
       <c r="G17" s="17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="H17" s="44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="45" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1899,8 +1985,8 @@
       <c r="C18" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>67</v>
+      <c r="D18" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>37</v>
@@ -1911,17 +1997,20 @@
       <c r="G18" s="15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="H18" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="46"/>
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>68</v>
+      <c r="D19" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>37</v>
@@ -1932,17 +2021,20 @@
       <c r="G19" s="16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="H19" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="46"/>
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>69</v>
+      <c r="D20" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>37</v>
@@ -1953,17 +2045,20 @@
       <c r="G20" s="16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
+      <c r="H20" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="47"/>
       <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>70</v>
+      <c r="D21" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>37</v>
@@ -1974,9 +2069,12 @@
       <c r="G21" s="17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
+      <c r="H21" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="45" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1985,8 +2083,8 @@
       <c r="C22" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>71</v>
+      <c r="D22" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>37</v>
@@ -1997,17 +2095,20 @@
       <c r="G22" s="15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="H22" s="43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="46"/>
       <c r="B23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>72</v>
+      <c r="D23" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>37</v>
@@ -2018,17 +2119,20 @@
       <c r="G23" s="16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="H23" s="43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="46"/>
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>73</v>
+      <c r="D24" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>37</v>
@@ -2039,30 +2143,36 @@
       <c r="G24" s="16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="46"/>
-      <c r="B25" s="39" t="s">
+      <c r="H24" s="43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="48"/>
+      <c r="B25" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="37" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+      <c r="H25" s="44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
         <v>80</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -2071,8 +2181,8 @@
       <c r="C26" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>74</v>
+      <c r="D26" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>37</v>
@@ -2083,17 +2193,20 @@
       <c r="G26" s="15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
+      <c r="H26" s="43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="46"/>
       <c r="B27" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>75</v>
+      <c r="D27" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>37</v>
@@ -2104,17 +2217,20 @@
       <c r="G27" s="16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="45"/>
+      <c r="H27" s="43" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="47"/>
       <c r="B28" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>76</v>
+      <c r="D28" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>37</v>
@@ -2125,60 +2241,14 @@
       <c r="G28" s="17" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="18"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="18"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="18"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="18"/>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="18"/>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D34" s="18"/>
-    </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D35" s="18"/>
-    </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="18"/>
-    </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="18"/>
-    </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="18"/>
-    </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D39" s="18"/>
-    </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D40" s="18"/>
+      <c r="H28" s="43" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G40" s="18" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D41" s="18"/>
-    </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D42" s="18"/>
-    </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D43" s="18"/>
-    </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D44" s="18"/>
-    </row>
-    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D45" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2199,8 +2269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18402DEB-E4E0-4F86-9553-AF55B8C5ECBF}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,13 +2281,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="39" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2228,7 +2298,7 @@
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="40" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2239,7 +2309,7 @@
       <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2250,7 +2320,7 @@
       <c r="B4" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2261,7 +2331,7 @@
       <c r="B5" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2272,7 +2342,7 @@
       <c r="B6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2283,7 +2353,7 @@
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2294,7 +2364,7 @@
       <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2305,7 +2375,7 @@
       <c r="B9" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2316,7 +2386,7 @@
       <c r="B10" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2327,7 +2397,7 @@
       <c r="B11" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2338,7 +2408,7 @@
       <c r="B12" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2349,7 +2419,7 @@
       <c r="B13" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2360,18 +2430,18 @@
       <c r="B14" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="40" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="41" t="s">
         <v>185</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2382,7 +2452,7 @@
       <c r="B16" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2393,7 +2463,7 @@
       <c r="B17" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2404,7 +2474,7 @@
       <c r="B18" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2415,7 +2485,7 @@
       <c r="B19" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2426,7 +2496,7 @@
       <c r="B20" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2437,7 +2507,7 @@
       <c r="B21" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2448,7 +2518,7 @@
       <c r="B22" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2459,7 +2529,7 @@
       <c r="B23" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2470,7 +2540,7 @@
       <c r="B24" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2481,7 +2551,7 @@
       <c r="B25" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="40" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2492,12 +2562,12 @@
       <c r="B26" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="40" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="35" t="s">
         <v>177</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -2519,7 +2589,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:B31"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,335 +2600,335 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="31"/>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="32" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="26" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="28" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="30" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="30" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="30" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="28" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="30" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="28" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="B31" s="47"/>
+      <c r="B31" s="49"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="24">
+      <c r="B34" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="24">
+      <c r="B36" s="23">
         <v>4</v>
       </c>
     </row>

</xml_diff>